<commit_message>
added saga to fetch desks
- modified response data to have deskGroupId property
</commit_message>
<xml_diff>
--- a/client/src/mock-data/bookings/SeatingArrangement.xlsx
+++ b/client/src/mock-data/bookings/SeatingArrangement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkburdip\Documents\SPark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hack-a-holicks\client\src\mock-data\bookings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444AE7B5-AD67-471C-B766-DD1FAEC673C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63597C2B-ACB7-49D5-87D3-1DD0D4F0F8C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="2595" windowWidth="18900" windowHeight="10980" xr2:uid="{C9B6A5A9-7B33-420C-9801-638D687A6860}"/>
+    <workbookView xWindow="-15480" yWindow="1950" windowWidth="15600" windowHeight="11160" xr2:uid="{C9B6A5A9-7B33-420C-9801-638D687A6860}"/>
   </bookViews>
   <sheets>
     <sheet name="Floor9" sheetId="1" r:id="rId1"/>
@@ -899,20 +899,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8245F3B2-83C8-4100-90B9-23F2197290D7}">
-  <dimension ref="B8:J21"/>
+  <dimension ref="B8:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,23 +920,23 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -948,150 +946,150 @@
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1109,9 +1107,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>56</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1149,7 +1147,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>64</v>
       </c>
@@ -1176,7 +1174,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1187,7 +1185,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>72</v>
       </c>
@@ -1214,7 +1212,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1225,7 +1223,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>80</v>
       </c>
@@ -1252,7 +1250,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1263,7 +1261,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1274,7 +1272,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>88</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1312,7 +1310,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>96</v>
       </c>
@@ -1339,7 +1337,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1350,7 +1348,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>104</v>
       </c>
@@ -1390,9 +1388,9 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>112</v>
       </c>
@@ -1419,7 +1417,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1430,7 +1428,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>120</v>
       </c>
@@ -1457,7 +1455,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1468,7 +1466,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>128</v>
       </c>
@@ -1495,7 +1493,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1506,7 +1504,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>136</v>
       </c>
@@ -1533,7 +1531,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1544,7 +1542,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1555,7 +1553,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>144</v>
       </c>
@@ -1582,7 +1580,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1593,7 +1591,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>152</v>
       </c>
@@ -1620,7 +1618,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1631,7 +1629,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>160</v>
       </c>

</xml_diff>